<commit_message>
created a working logging in and logging out function
</commit_message>
<xml_diff>
--- a/Data/Users.xlsx
+++ b/Data/Users.xlsx
@@ -67,22 +67,19 @@
     <x:t>USER002</x:t>
   </x:si>
   <x:si>
-    <x:t>Adib</x:t>
-  </x:si>
-  <x:si>
-    <x:t>AdibMohamad</x:t>
+    <x:t>adib</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Operator</x:t>
   </x:si>
   <x:si>
     <x:t>USER003</x:t>
   </x:si>
   <x:si>
-    <x:t>Test</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TestTest</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Operator</x:t>
+    <x:t>adibsv</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Supervisor</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -470,12 +467,12 @@
     <x:col min="2" max="2" width="9.996339" style="0" customWidth="1"/>
     <x:col min="3" max="3" width="9.710625" style="0" customWidth="1"/>
     <x:col min="4" max="4" width="20.424911" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="9.139196" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="10.424911" style="0" customWidth="1"/>
     <x:col min="6" max="6" width="7.853482" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="16.282054" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="15.282054" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="16.710625" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="14.853482" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="15.282054" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="14.282054" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:10" s="1" customFormat="1">
@@ -530,16 +527,16 @@
         <x:v>1</x:v>
       </x:c>
       <x:c r="G2" s="2">
-        <x:v>45950.5003837037</x:v>
+        <x:v>45965.6871277315</x:v>
       </x:c>
       <x:c r="H2" s="2">
-        <x:v>45950.5003837037</x:v>
+        <x:v>45965.6871277315</x:v>
       </x:c>
       <x:c r="I2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
       <x:c r="J2" s="2">
-        <x:v>45964.7436500694</x:v>
+        <x:v>45966.4101940394</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -553,22 +550,25 @@
         <x:v>17</x:v>
       </x:c>
       <x:c r="D3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
         <x:v>18</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>14</x:v>
       </x:c>
       <x:c r="F3" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="G3" s="2">
-        <x:v>45950.5007225926</x:v>
+        <x:v>45965.7040329398</x:v>
       </x:c>
       <x:c r="H3" s="2">
-        <x:v>45950.5007225926</x:v>
+        <x:v>45965.7040329398</x:v>
       </x:c>
       <x:c r="I3" s="0" t="s">
         <x:v>11</x:v>
+      </x:c>
+      <x:c r="J3" s="2">
+        <x:v>45966.4106425926</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
@@ -582,22 +582,25 @@
         <x:v>20</x:v>
       </x:c>
       <x:c r="D4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
         <x:v>21</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>22</x:v>
       </x:c>
       <x:c r="F4" s="0" t="b">
         <x:v>1</x:v>
       </x:c>
       <x:c r="G4" s="2">
-        <x:v>45950.5052933449</x:v>
+        <x:v>45965.7242735764</x:v>
       </x:c>
       <x:c r="H4" s="2">
-        <x:v>45950.5052933449</x:v>
+        <x:v>45965.7242735764</x:v>
       </x:c>
       <x:c r="I4" s="0" t="s">
         <x:v>11</x:v>
+      </x:c>
+      <x:c r="J4" s="2">
+        <x:v>45966.4104202546</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
changing weighing and dashboard
</commit_message>
<xml_diff>
--- a/Data/Users.xlsx
+++ b/Data/Users.xlsx
@@ -536,7 +536,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="J2" s="2">
-        <x:v>45966.4738045602</x:v>
+        <x:v>45966.5290898611</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -568,7 +568,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="J3" s="2">
-        <x:v>45966.5204188657</x:v>
+        <x:v>45967.3909744329</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
@@ -600,7 +600,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="J4" s="2">
-        <x:v>45966.5186435185</x:v>
+        <x:v>45967.3797240509</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
optimize the autologout features, added the ingredient usage report
</commit_message>
<xml_diff>
--- a/Data/Users.xlsx
+++ b/Data/Users.xlsx
@@ -472,7 +472,7 @@
     <x:col min="7" max="7" width="15.282054" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="16.710625" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="14.853482" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="15.282054" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="16.282054" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:10" s="1" customFormat="1">
@@ -536,7 +536,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="J2" s="2">
-        <x:v>45968.526453287</x:v>
+        <x:v>45972.5061416551</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -568,7 +568,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="J3" s="2">
-        <x:v>45972.4069968403</x:v>
+        <x:v>45972.5019591319</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">

</xml_diff>

<commit_message>
Finalized Version ready for Publishing
</commit_message>
<xml_diff>
--- a/Data/Users.xlsx
+++ b/Data/Users.xlsx
@@ -472,7 +472,7 @@
     <x:col min="7" max="7" width="15.282054" style="0" customWidth="1"/>
     <x:col min="8" max="8" width="16.710625" style="0" customWidth="1"/>
     <x:col min="9" max="9" width="14.853482" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="16.282054" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="15.282054" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:10" s="1" customFormat="1">
@@ -536,7 +536,7 @@
         <x:v>15</x:v>
       </x:c>
       <x:c r="J2" s="2">
-        <x:v>45972.5114840162</x:v>
+        <x:v>45973.3999544907</x:v>
       </x:c>
     </x:row>
     <x:row r="3" spans="1:10">
@@ -568,7 +568,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="J3" s="2">
-        <x:v>45972.5019591319</x:v>
+        <x:v>45973.411712419</x:v>
       </x:c>
     </x:row>
     <x:row r="4" spans="1:10">
@@ -600,7 +600,7 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="J4" s="2">
-        <x:v>45968.6448414468</x:v>
+        <x:v>45973.3890095949</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>